<commit_message>
課題 . 6 FizzBuzz if文の追加
</commit_message>
<xml_diff>
--- a/研修記録.xlsx
+++ b/研修記録.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPOS#195\Desktop\新人研修\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FE7CBA-AA48-4E8B-8FEB-0B13124B3548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73169DCD-6A72-4D80-A90E-BFBA44926AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="-15390" windowWidth="27330" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>